<commit_message>
Added variable layer for PSO
</commit_message>
<xml_diff>
--- a/Pythia/SentimentAnalysis/cnn_scrape_polarity.xlsx
+++ b/Pythia/SentimentAnalysis/cnn_scrape_polarity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brandon\Desktop\GitHub Links\HPT-OASiS\Pythia\SentimentAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8FD63E-3F57-4D71-BAA1-95A5902CC7DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{546BE70F-B14A-4F47-BA0F-33518A3BD30C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9000" yWindow="3000" windowWidth="13632" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -196,37 +196,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -254,36 +224,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -962,13 +902,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C1048576">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>